<commit_message>
[feat/ch1146] updated import models
</commit_message>
<xml_diff>
--- a/client/public/static/documents/import_model_en.xlsx
+++ b/client/public/static/documents/import_model_en.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianorodriguez/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianorodriguez/git/parallel/client/public/static/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC67B127-3DFA-6D49-9C2E-1DB7F9BBB76D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2482F9F5-013D-814D-8FB2-A0C004B2AD94}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{E7C17285-F5ED-3A43-ADB5-68BFE6124626}"/>
   </bookViews>
@@ -34,45 +34,87 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="13">
-  <si>
-    <t>Comunidad</t>
-  </si>
-  <si>
-    <t>Provincia</t>
-  </si>
-  <si>
-    <t>Andalucía</t>
-  </si>
-  <si>
-    <t>Almeria</t>
-  </si>
-  <si>
-    <t>Cadiz</t>
-  </si>
-  <si>
-    <t>Cordoba</t>
-  </si>
-  <si>
-    <t>Aragón</t>
-  </si>
-  <si>
-    <t>Huesca</t>
-  </si>
-  <si>
-    <t>Teruel</t>
-  </si>
-  <si>
-    <t>Zaragoza</t>
-  </si>
-  <si>
-    <t>Canarias</t>
-  </si>
-  <si>
-    <t>Palmas</t>
-  </si>
-  <si>
-    <t>Tenerife</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>Los Angeles</t>
+  </si>
+  <si>
+    <t>Sacramento</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t>Houston</t>
+  </si>
+  <si>
+    <t>San Diego</t>
+  </si>
+  <si>
+    <t>San Francisco</t>
+  </si>
+  <si>
+    <t>Death Valley</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>Jacksonville</t>
+  </si>
+  <si>
+    <t>Miami</t>
+  </si>
+  <si>
+    <t>Orlando</t>
+  </si>
+  <si>
+    <t>Tampa</t>
+  </si>
+  <si>
+    <t>Illinois</t>
+  </si>
+  <si>
+    <t>Cairo</t>
+  </si>
+  <si>
+    <t>Chicago</t>
+  </si>
+  <si>
+    <t>Rockford</t>
+  </si>
+  <si>
+    <t>Springfield</t>
+  </si>
+  <si>
+    <t>Nevada</t>
+  </si>
+  <si>
+    <t>Las Vegas</t>
+  </si>
+  <si>
+    <t>Reno</t>
+  </si>
+  <si>
+    <t>Carson City</t>
+  </si>
+  <si>
+    <t>El Paso</t>
+  </si>
+  <si>
+    <t>Brownsville</t>
+  </si>
+  <si>
+    <t>Dallas</t>
   </si>
 </sst>
 </file>
@@ -433,15 +475,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF7A90B7-597E-B04A-A208-35AE2523E761}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -468,7 +511,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E3" s="1"/>
     </row>
@@ -477,7 +520,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E4" s="1"/>
     </row>
@@ -495,25 +538,25 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E8" s="1"/>
     </row>
@@ -522,7 +565,7 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E9" s="1"/>
     </row>
@@ -531,81 +574,105 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>